<commit_message>
added script for presentation
</commit_message>
<xml_diff>
--- a/business plan/Cash Flow.xlsx
+++ b/business plan/Cash Flow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-6700" yWindow="-24440" windowWidth="37220" windowHeight="22700" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Financial Forecast" sheetId="1" r:id="rId1"/>
@@ -302,7 +302,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -634,8 +634,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="94">
+  <cellStyleXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -730,8 +748,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -954,6 +976,42 @@
     <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="9" borderId="21" xfId="63" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="9" borderId="15" xfId="63" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="9" borderId="22" xfId="63" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="9" borderId="25" xfId="63" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -984,44 +1042,17 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="9" borderId="21" xfId="63" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="9" borderId="15" xfId="63" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="9" borderId="22" xfId="63" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="9" borderId="25" xfId="63" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="94">
+  <cellStyles count="98">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1068,6 +1099,8 @@
     <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1114,6 +1147,8 @@
     <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="63" builtinId="10"/>
   </cellStyles>
@@ -1465,11 +1500,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:AM29"/>
+  <dimension ref="A1:AM30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C37" sqref="C37"/>
+      <pane xSplit="2" topLeftCell="AF1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1483,7 +1518,7 @@
     <row r="1" spans="1:39" s="64" customFormat="1" ht="30" customHeight="1">
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="77" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="58">
@@ -1602,51 +1637,51 @@
       <c r="B2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="88" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="77" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="77" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="S2" s="78"/>
-      <c r="T2" s="78"/>
-      <c r="U2" s="78"/>
-      <c r="V2" s="78"/>
-      <c r="W2" s="78"/>
-      <c r="X2" s="78"/>
-      <c r="Y2" s="78"/>
-      <c r="Z2" s="78"/>
-      <c r="AA2" s="79"/>
-      <c r="AB2" s="77" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="78"/>
-      <c r="AD2" s="78"/>
-      <c r="AE2" s="78"/>
-      <c r="AF2" s="78"/>
-      <c r="AG2" s="78"/>
-      <c r="AH2" s="78"/>
-      <c r="AI2" s="78"/>
-      <c r="AJ2" s="78"/>
-      <c r="AK2" s="78"/>
-      <c r="AL2" s="78"/>
-      <c r="AM2" s="79"/>
+      <c r="C2" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="89" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="89" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="90"/>
+      <c r="S2" s="90"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="90"/>
+      <c r="V2" s="90"/>
+      <c r="W2" s="90"/>
+      <c r="X2" s="90"/>
+      <c r="Y2" s="90"/>
+      <c r="Z2" s="90"/>
+      <c r="AA2" s="91"/>
+      <c r="AB2" s="89" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="90"/>
+      <c r="AD2" s="90"/>
+      <c r="AE2" s="90"/>
+      <c r="AF2" s="90"/>
+      <c r="AG2" s="90"/>
+      <c r="AH2" s="90"/>
+      <c r="AI2" s="90"/>
+      <c r="AJ2" s="90"/>
+      <c r="AK2" s="90"/>
+      <c r="AL2" s="90"/>
+      <c r="AM2" s="91"/>
     </row>
     <row r="3" spans="1:39" s="67" customFormat="1">
       <c r="A3" s="1" t="s">
@@ -1655,7 +1690,7 @@
       <c r="B3" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="89"/>
+      <c r="C3" s="79"/>
       <c r="D3" s="24">
         <v>500</v>
       </c>
@@ -1772,7 +1807,7 @@
       <c r="B4" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="89"/>
+      <c r="C4" s="79"/>
       <c r="D4" s="24">
         <v>0</v>
       </c>
@@ -1889,7 +1924,7 @@
       <c r="B5" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="89"/>
+      <c r="C5" s="79"/>
       <c r="D5" s="24">
         <v>0</v>
       </c>
@@ -2006,7 +2041,7 @@
       <c r="B6" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="89"/>
+      <c r="C6" s="79"/>
       <c r="D6" s="24">
         <v>0</v>
       </c>
@@ -2123,7 +2158,7 @@
       <c r="B7" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="89">
+      <c r="C7" s="79">
         <v>900</v>
       </c>
       <c r="D7" s="24"/>
@@ -2168,7 +2203,7 @@
       <c r="B8" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="90">
+      <c r="C8" s="80">
         <f>SUM(C3:C7)</f>
         <v>900</v>
       </c>
@@ -2322,51 +2357,51 @@
       <c r="B9" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="91" t="s">
+      <c r="C9" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="74" t="s">
+      <c r="D9" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="76"/>
-      <c r="P9" s="74" t="s">
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="87"/>
+      <c r="J9" s="87"/>
+      <c r="K9" s="87"/>
+      <c r="L9" s="87"/>
+      <c r="M9" s="87"/>
+      <c r="N9" s="87"/>
+      <c r="O9" s="88"/>
+      <c r="P9" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="Q9" s="75"/>
-      <c r="R9" s="75"/>
-      <c r="S9" s="75"/>
-      <c r="T9" s="75"/>
-      <c r="U9" s="75"/>
-      <c r="V9" s="75"/>
-      <c r="W9" s="75"/>
-      <c r="X9" s="75"/>
-      <c r="Y9" s="75"/>
-      <c r="Z9" s="75"/>
-      <c r="AA9" s="76"/>
-      <c r="AB9" s="74" t="s">
+      <c r="Q9" s="87"/>
+      <c r="R9" s="87"/>
+      <c r="S9" s="87"/>
+      <c r="T9" s="87"/>
+      <c r="U9" s="87"/>
+      <c r="V9" s="87"/>
+      <c r="W9" s="87"/>
+      <c r="X9" s="87"/>
+      <c r="Y9" s="87"/>
+      <c r="Z9" s="87"/>
+      <c r="AA9" s="88"/>
+      <c r="AB9" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="AC9" s="75"/>
-      <c r="AD9" s="75"/>
-      <c r="AE9" s="75"/>
-      <c r="AF9" s="75"/>
-      <c r="AG9" s="75"/>
-      <c r="AH9" s="75"/>
-      <c r="AI9" s="75"/>
-      <c r="AJ9" s="75"/>
-      <c r="AK9" s="75"/>
-      <c r="AL9" s="75"/>
-      <c r="AM9" s="76"/>
+      <c r="AC9" s="87"/>
+      <c r="AD9" s="87"/>
+      <c r="AE9" s="87"/>
+      <c r="AF9" s="87"/>
+      <c r="AG9" s="87"/>
+      <c r="AH9" s="87"/>
+      <c r="AI9" s="87"/>
+      <c r="AJ9" s="87"/>
+      <c r="AK9" s="87"/>
+      <c r="AL9" s="87"/>
+      <c r="AM9" s="88"/>
     </row>
     <row r="10" spans="1:39" s="70" customFormat="1">
       <c r="A10" s="5" t="s">
@@ -2375,7 +2410,7 @@
       <c r="B10" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="92"/>
+      <c r="C10" s="82"/>
       <c r="D10" s="28">
         <v>108</v>
       </c>
@@ -2490,7 +2525,7 @@
       <c r="B11" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="92"/>
+      <c r="C11" s="82"/>
       <c r="D11" s="28">
         <v>65</v>
       </c>
@@ -2607,7 +2642,7 @@
       <c r="B12" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="92">
+      <c r="C12" s="82">
         <v>60.8</v>
       </c>
       <c r="D12" s="28">
@@ -2726,7 +2761,7 @@
       <c r="B13" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="92"/>
+      <c r="C13" s="82"/>
       <c r="D13" s="28">
         <v>17</v>
       </c>
@@ -2843,7 +2878,7 @@
       <c r="B14" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="92">
+      <c r="C14" s="82">
         <v>7</v>
       </c>
       <c r="D14" s="28"/>
@@ -2890,7 +2925,7 @@
       <c r="B15" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="92"/>
+      <c r="C15" s="82"/>
       <c r="D15" s="28">
         <f>SUM((46.88*3)+6)</f>
         <v>146.64000000000001</v>
@@ -3043,7 +3078,7 @@
       <c r="B16" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="92"/>
+      <c r="C16" s="82"/>
       <c r="D16" s="28">
         <v>0</v>
       </c>
@@ -3160,7 +3195,7 @@
       <c r="B17" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="92">
+      <c r="C17" s="82">
         <v>11.5</v>
       </c>
       <c r="D17" s="28">
@@ -3277,7 +3312,7 @@
       <c r="B18" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="92"/>
+      <c r="C18" s="82"/>
       <c r="D18" s="28"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -3288,11 +3323,11 @@
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="29"/>
-      <c r="P18" s="28">
+      <c r="N18" s="96"/>
+      <c r="O18" s="98">
         <v>1000</v>
       </c>
+      <c r="P18" s="97"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
@@ -3304,19 +3339,17 @@
       <c r="W18" s="6"/>
       <c r="X18" s="6"/>
       <c r="Y18" s="6"/>
-      <c r="Z18" s="6"/>
-      <c r="AA18" s="29"/>
-      <c r="AB18" s="28">
+      <c r="Z18" s="96"/>
+      <c r="AA18" s="98">
         <v>10000</v>
       </c>
+      <c r="AB18" s="97"/>
       <c r="AC18" s="6"/>
       <c r="AD18" s="6"/>
       <c r="AE18" s="6"/>
       <c r="AF18" s="6"/>
       <c r="AG18" s="6"/>
-      <c r="AH18" s="6">
-        <v>10000</v>
-      </c>
+      <c r="AH18" s="6"/>
       <c r="AI18" s="6"/>
       <c r="AJ18" s="6"/>
       <c r="AK18" s="6"/>
@@ -3330,7 +3363,7 @@
       <c r="B19" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="92">
+      <c r="C19" s="82">
         <v>50</v>
       </c>
       <c r="D19" s="28"/>
@@ -3377,7 +3410,7 @@
       <c r="B20" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="92"/>
+      <c r="C20" s="82"/>
       <c r="D20" s="28">
         <v>25</v>
       </c>
@@ -3494,7 +3527,7 @@
       <c r="B21" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="92">
+      <c r="C21" s="82">
         <v>10</v>
       </c>
       <c r="D21" s="28"/>
@@ -3541,7 +3574,7 @@
       <c r="B22" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="92"/>
+      <c r="C22" s="82"/>
       <c r="D22" s="28">
         <v>48.79</v>
       </c>
@@ -3658,7 +3691,7 @@
       <c r="B23" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="92"/>
+      <c r="C23" s="82"/>
       <c r="D23" s="63"/>
       <c r="E23" s="73"/>
       <c r="F23" s="73"/>
@@ -3707,21 +3740,21 @@
       <c r="B24" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="93">
+      <c r="C24" s="83">
         <v>500</v>
       </c>
-      <c r="D24" s="84"/>
-      <c r="E24" s="85"/>
-      <c r="F24" s="85"/>
-      <c r="G24" s="85"/>
-      <c r="H24" s="85"/>
-      <c r="I24" s="85"/>
-      <c r="J24" s="85"/>
-      <c r="K24" s="85"/>
-      <c r="L24" s="85"/>
-      <c r="M24" s="85"/>
-      <c r="N24" s="85"/>
-      <c r="O24" s="86"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="75"/>
+      <c r="J24" s="75"/>
+      <c r="K24" s="75"/>
+      <c r="L24" s="75"/>
+      <c r="M24" s="75"/>
+      <c r="N24" s="75"/>
+      <c r="O24" s="76"/>
       <c r="P24" s="63"/>
       <c r="Q24" s="73"/>
       <c r="R24" s="73"/>
@@ -3752,7 +3785,7 @@
       <c r="B25" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="92"/>
+      <c r="C25" s="82"/>
       <c r="D25" s="63"/>
       <c r="E25" s="73"/>
       <c r="F25" s="73"/>
@@ -3796,579 +3829,626 @@
     </row>
     <row r="26" spans="1:39" s="70" customFormat="1">
       <c r="A26" s="5"/>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="37"/>
+      <c r="C26" s="82"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="73"/>
+      <c r="I26" s="73"/>
+      <c r="J26" s="73"/>
+      <c r="K26" s="73"/>
+      <c r="L26" s="73"/>
+      <c r="M26" s="73"/>
+      <c r="N26" s="73"/>
+      <c r="O26" s="71"/>
+      <c r="P26" s="63">
+        <f>SUM(0.4*O30)</f>
+        <v>1557.6159999999998</v>
+      </c>
+      <c r="Q26" s="73"/>
+      <c r="R26" s="73"/>
+      <c r="S26" s="73"/>
+      <c r="T26" s="73"/>
+      <c r="U26" s="73"/>
+      <c r="V26" s="73"/>
+      <c r="W26" s="73"/>
+      <c r="X26" s="73"/>
+      <c r="Y26" s="73"/>
+      <c r="Z26" s="73"/>
+      <c r="AA26" s="71"/>
+      <c r="AB26" s="63">
+        <f>SUM(0.4*AA30)</f>
+        <v>6647.9455999999964</v>
+      </c>
+      <c r="AC26" s="73"/>
+      <c r="AD26" s="73"/>
+      <c r="AE26" s="73"/>
+      <c r="AF26" s="73"/>
+      <c r="AG26" s="73"/>
+      <c r="AH26" s="73"/>
+      <c r="AI26" s="73"/>
+      <c r="AJ26" s="73"/>
+      <c r="AK26" s="73"/>
+      <c r="AL26" s="73"/>
+      <c r="AM26" s="71"/>
+    </row>
+    <row r="27" spans="1:39" s="70" customFormat="1">
+      <c r="A27" s="5"/>
+      <c r="B27" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="92"/>
-      <c r="D26" s="28">
-        <v>0</v>
-      </c>
-      <c r="E26" s="6">
-        <v>0</v>
-      </c>
-      <c r="F26" s="6">
+      <c r="C27" s="82"/>
+      <c r="D27" s="28">
+        <v>0</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0</v>
+      </c>
+      <c r="F27" s="6">
         <v>2700</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G27" s="6">
         <v>2700</v>
       </c>
-      <c r="H26" s="6">
+      <c r="H27" s="6">
         <v>2700</v>
       </c>
-      <c r="I26" s="6">
+      <c r="I27" s="6">
         <v>2700</v>
       </c>
-      <c r="J26" s="6">
+      <c r="J27" s="6">
         <v>2700</v>
       </c>
-      <c r="K26" s="6">
+      <c r="K27" s="6">
         <v>2700</v>
       </c>
-      <c r="L26" s="6">
+      <c r="L27" s="6">
         <v>2700</v>
       </c>
-      <c r="M26" s="6">
+      <c r="M27" s="6">
         <v>2700</v>
       </c>
-      <c r="N26" s="6">
+      <c r="N27" s="6">
         <v>2700</v>
       </c>
-      <c r="O26" s="29">
+      <c r="O27" s="29">
         <v>2700</v>
       </c>
-      <c r="P26" s="63">
+      <c r="P27" s="63">
         <v>4500</v>
       </c>
-      <c r="Q26" s="73">
+      <c r="Q27" s="73">
         <v>4500</v>
       </c>
-      <c r="R26" s="73">
+      <c r="R27" s="73">
         <v>4500</v>
       </c>
-      <c r="S26" s="73">
+      <c r="S27" s="73">
         <v>4500</v>
       </c>
-      <c r="T26" s="73">
+      <c r="T27" s="73">
         <v>4500</v>
       </c>
-      <c r="U26" s="73">
+      <c r="U27" s="73">
         <v>4500</v>
       </c>
-      <c r="V26" s="73">
+      <c r="V27" s="73">
         <v>4500</v>
       </c>
-      <c r="W26" s="73">
+      <c r="W27" s="73">
         <v>4500</v>
       </c>
-      <c r="X26" s="73">
+      <c r="X27" s="73">
         <v>4500</v>
       </c>
-      <c r="Y26" s="73">
+      <c r="Y27" s="73">
         <v>4500</v>
       </c>
-      <c r="Z26" s="73">
+      <c r="Z27" s="73">
         <v>4500</v>
       </c>
-      <c r="AA26" s="71">
+      <c r="AA27" s="71">
         <v>4500</v>
       </c>
-      <c r="AB26" s="73">
+      <c r="AB27" s="63">
         <v>9500</v>
       </c>
-      <c r="AC26" s="73">
+      <c r="AC27" s="73">
         <v>9500</v>
       </c>
-      <c r="AD26" s="73">
+      <c r="AD27" s="73">
         <v>9500</v>
       </c>
-      <c r="AE26" s="73">
+      <c r="AE27" s="73">
         <v>9500</v>
       </c>
-      <c r="AF26" s="73">
+      <c r="AF27" s="73">
         <v>9500</v>
       </c>
-      <c r="AG26" s="73">
+      <c r="AG27" s="73">
         <v>9500</v>
       </c>
-      <c r="AH26" s="73">
+      <c r="AH27" s="73">
         <v>9500</v>
       </c>
-      <c r="AI26" s="73">
+      <c r="AI27" s="73">
         <v>9500</v>
       </c>
-      <c r="AJ26" s="73">
+      <c r="AJ27" s="73">
         <v>9500</v>
       </c>
-      <c r="AK26" s="73">
+      <c r="AK27" s="73">
         <v>9500</v>
       </c>
-      <c r="AL26" s="73">
+      <c r="AL27" s="73">
         <v>9500</v>
       </c>
-      <c r="AM26" s="73">
+      <c r="AM27" s="71">
         <v>9500</v>
       </c>
     </row>
-    <row r="27" spans="1:39" s="72" customFormat="1" ht="30" customHeight="1">
-      <c r="A27" s="7"/>
-      <c r="B27" s="36" t="s">
+    <row r="28" spans="1:39" s="72" customFormat="1" ht="30" customHeight="1">
+      <c r="A28" s="7"/>
+      <c r="B28" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="90">
-        <f t="shared" ref="C27:O27" si="2">SUM(C9:C26)</f>
+      <c r="C28" s="80">
+        <f t="shared" ref="C28:O28" si="2">SUM(C9:C27)</f>
         <v>639.29999999999995</v>
       </c>
-      <c r="D27" s="26">
+      <c r="D28" s="26">
         <f t="shared" si="2"/>
         <v>482.73000000000008</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E28" s="8">
         <f t="shared" si="2"/>
         <v>492.63000000000005</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F28" s="8">
         <f t="shared" si="2"/>
         <v>3192.63</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G28" s="8">
         <f t="shared" si="2"/>
         <v>3192.63</v>
       </c>
-      <c r="H27" s="8">
+      <c r="H28" s="8">
         <f t="shared" si="2"/>
         <v>3192.63</v>
       </c>
-      <c r="I27" s="8">
+      <c r="I28" s="8">
         <f t="shared" si="2"/>
         <v>3192.63</v>
       </c>
-      <c r="J27" s="8">
+      <c r="J28" s="8">
         <f t="shared" si="2"/>
         <v>3192.63</v>
       </c>
-      <c r="K27" s="8">
+      <c r="K28" s="8">
         <f t="shared" si="2"/>
         <v>3192.63</v>
       </c>
-      <c r="L27" s="8">
+      <c r="L28" s="8">
         <f t="shared" si="2"/>
         <v>3192.63</v>
       </c>
-      <c r="M27" s="8">
+      <c r="M28" s="8">
         <f t="shared" si="2"/>
         <v>3192.63</v>
       </c>
-      <c r="N27" s="8">
+      <c r="N28" s="8">
         <f t="shared" si="2"/>
         <v>3192.63</v>
       </c>
-      <c r="O27" s="27">
+      <c r="O28" s="27">
         <f t="shared" si="2"/>
-        <v>4057.63</v>
-      </c>
-      <c r="P27" s="26">
-        <f t="shared" ref="P27" si="3">SUM(P9:P26)</f>
-        <v>6087.63</v>
-      </c>
-      <c r="Q27" s="8">
-        <f t="shared" ref="Q27" si="4">SUM(Q9:Q26)</f>
+        <v>5057.63</v>
+      </c>
+      <c r="P28" s="26">
+        <f t="shared" ref="P28" si="3">SUM(P9:P27)</f>
+        <v>6645.2459999999992</v>
+      </c>
+      <c r="Q28" s="8">
+        <f t="shared" ref="Q28" si="4">SUM(Q9:Q27)</f>
         <v>5087.63</v>
       </c>
-      <c r="R27" s="8">
-        <f t="shared" ref="R27" si="5">SUM(R9:R26)</f>
+      <c r="R28" s="8">
+        <f t="shared" ref="R28" si="5">SUM(R9:R27)</f>
         <v>5087.63</v>
       </c>
-      <c r="S27" s="8">
-        <f t="shared" ref="S27" si="6">SUM(S9:S26)</f>
+      <c r="S28" s="8">
+        <f t="shared" ref="S28" si="6">SUM(S9:S27)</f>
         <v>5087.63</v>
       </c>
-      <c r="T27" s="8">
-        <f t="shared" ref="T27" si="7">SUM(T9:T26)</f>
+      <c r="T28" s="8">
+        <f t="shared" ref="T28" si="7">SUM(T9:T27)</f>
         <v>5087.63</v>
       </c>
-      <c r="U27" s="8">
-        <f t="shared" ref="U27" si="8">SUM(U9:U26)</f>
+      <c r="U28" s="8">
+        <f t="shared" ref="U28" si="8">SUM(U9:U27)</f>
         <v>5087.63</v>
       </c>
-      <c r="V27" s="8">
-        <f t="shared" ref="V27" si="9">SUM(V9:V26)</f>
+      <c r="V28" s="8">
+        <f t="shared" ref="V28" si="9">SUM(V9:V27)</f>
         <v>10087.630000000001</v>
       </c>
-      <c r="W27" s="8">
-        <f t="shared" ref="W27" si="10">SUM(W9:W26)</f>
+      <c r="W28" s="8">
+        <f t="shared" ref="W28" si="10">SUM(W9:W27)</f>
         <v>5087.63</v>
       </c>
-      <c r="X27" s="8">
-        <f t="shared" ref="X27" si="11">SUM(X9:X26)</f>
+      <c r="X28" s="8">
+        <f t="shared" ref="X28" si="11">SUM(X9:X27)</f>
         <v>5087.63</v>
       </c>
-      <c r="Y27" s="8">
-        <f t="shared" ref="Y27" si="12">SUM(Y9:Y26)</f>
+      <c r="Y28" s="8">
+        <f t="shared" ref="Y28" si="12">SUM(Y9:Y27)</f>
         <v>5087.63</v>
       </c>
-      <c r="Z27" s="8">
-        <f t="shared" ref="Z27" si="13">SUM(Z9:Z26)</f>
+      <c r="Z28" s="8">
+        <f t="shared" ref="Z28" si="13">SUM(Z9:Z27)</f>
         <v>5087.63</v>
       </c>
-      <c r="AA27" s="27">
-        <f t="shared" ref="AA27" si="14">SUM(AA9:AA26)</f>
-        <v>5952.63</v>
-      </c>
-      <c r="AB27" s="26">
-        <f t="shared" ref="AB27" si="15">SUM(AB9:AB26)</f>
-        <v>20087.63</v>
-      </c>
-      <c r="AC27" s="8">
-        <f t="shared" ref="AC27" si="16">SUM(AC9:AC26)</f>
+      <c r="AA28" s="27">
+        <f t="shared" ref="AA28" si="14">SUM(AA9:AA27)</f>
+        <v>15952.630000000001</v>
+      </c>
+      <c r="AB28" s="26">
+        <f t="shared" ref="AB28" si="15">SUM(AB9:AB27)</f>
+        <v>16735.575599999996</v>
+      </c>
+      <c r="AC28" s="8">
+        <f t="shared" ref="AC28" si="16">SUM(AC9:AC27)</f>
         <v>10087.629999999999</v>
       </c>
-      <c r="AD27" s="8">
-        <f t="shared" ref="AD27" si="17">SUM(AD9:AD26)</f>
+      <c r="AD28" s="8">
+        <f t="shared" ref="AD28" si="17">SUM(AD9:AD27)</f>
         <v>10087.629999999999</v>
       </c>
-      <c r="AE27" s="8">
-        <f t="shared" ref="AE27" si="18">SUM(AE9:AE26)</f>
+      <c r="AE28" s="8">
+        <f t="shared" ref="AE28" si="18">SUM(AE9:AE27)</f>
         <v>10087.629999999999</v>
       </c>
-      <c r="AF27" s="8">
-        <f t="shared" ref="AF27" si="19">SUM(AF9:AF26)</f>
+      <c r="AF28" s="8">
+        <f t="shared" ref="AF28" si="19">SUM(AF9:AF27)</f>
         <v>10087.629999999999</v>
       </c>
-      <c r="AG27" s="8">
-        <f t="shared" ref="AG27" si="20">SUM(AG9:AG26)</f>
+      <c r="AG28" s="8">
+        <f t="shared" ref="AG28" si="20">SUM(AG9:AG27)</f>
         <v>10087.629999999999</v>
       </c>
-      <c r="AH27" s="8">
-        <f t="shared" ref="AH27" si="21">SUM(AH9:AH26)</f>
-        <v>20087.63</v>
-      </c>
-      <c r="AI27" s="8">
-        <f t="shared" ref="AI27" si="22">SUM(AI9:AI26)</f>
+      <c r="AH28" s="8">
+        <f t="shared" ref="AH28" si="21">SUM(AH9:AH27)</f>
         <v>10087.629999999999</v>
       </c>
-      <c r="AJ27" s="8">
-        <f t="shared" ref="AJ27" si="23">SUM(AJ9:AJ26)</f>
+      <c r="AI28" s="8">
+        <f t="shared" ref="AI28" si="22">SUM(AI9:AI27)</f>
         <v>10087.629999999999</v>
       </c>
-      <c r="AK27" s="8">
-        <f t="shared" ref="AK27" si="24">SUM(AK9:AK26)</f>
+      <c r="AJ28" s="8">
+        <f t="shared" ref="AJ28" si="23">SUM(AJ9:AJ27)</f>
         <v>10087.629999999999</v>
       </c>
-      <c r="AL27" s="8">
-        <f t="shared" ref="AL27" si="25">SUM(AL9:AL26)</f>
+      <c r="AK28" s="8">
+        <f t="shared" ref="AK28" si="24">SUM(AK9:AK27)</f>
         <v>10087.629999999999</v>
       </c>
-      <c r="AM27" s="27">
-        <f t="shared" ref="AM27" si="26">SUM(AM9:AM26)</f>
+      <c r="AL28" s="8">
+        <f t="shared" ref="AL28" si="25">SUM(AL9:AL27)</f>
+        <v>10087.629999999999</v>
+      </c>
+      <c r="AM28" s="27">
+        <f t="shared" ref="AM28" si="26">SUM(AM9:AM27)</f>
         <v>10502.63</v>
       </c>
     </row>
-    <row r="28" spans="1:39">
-      <c r="A28" s="2"/>
-      <c r="B28" s="38" t="s">
+    <row r="29" spans="1:39">
+      <c r="A29" s="2"/>
+      <c r="B29" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="94">
-        <f t="shared" ref="C28:O28" si="27">C8-C27</f>
+      <c r="C29" s="84">
+        <f t="shared" ref="C29:O29" si="27">C8-C28</f>
         <v>260.70000000000005</v>
       </c>
-      <c r="D28" s="30">
+      <c r="D29" s="30">
         <f t="shared" si="27"/>
         <v>17.269999999999925</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E29" s="3">
         <f t="shared" si="27"/>
         <v>1107.3699999999999</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F29" s="3">
         <f t="shared" si="27"/>
         <v>-792.63000000000011</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G29" s="3">
         <f t="shared" si="27"/>
         <v>-92.630000000000109</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H29" s="3">
         <f t="shared" si="27"/>
         <v>407.36999999999989</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I29" s="3">
         <f t="shared" si="27"/>
         <v>407.36999999999989</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J29" s="3">
         <f t="shared" si="27"/>
         <v>407.36999999999989</v>
       </c>
-      <c r="K28" s="3">
+      <c r="K29" s="3">
         <f t="shared" si="27"/>
         <v>607.36999999999989</v>
       </c>
-      <c r="L28" s="3">
+      <c r="L29" s="3">
         <f t="shared" si="27"/>
         <v>807.36999999999989</v>
       </c>
-      <c r="M28" s="3">
+      <c r="M29" s="3">
         <f t="shared" si="27"/>
         <v>707.36999999999989</v>
       </c>
-      <c r="N28" s="3">
+      <c r="N29" s="3">
         <f t="shared" si="27"/>
         <v>807.36999999999989</v>
       </c>
-      <c r="O28" s="31">
+      <c r="O29" s="31">
         <f t="shared" si="27"/>
-        <v>242.36999999999989</v>
-      </c>
-      <c r="P28" s="30">
-        <f t="shared" ref="P28" si="28">P8-P27</f>
-        <v>-137.63000000000011</v>
-      </c>
-      <c r="Q28" s="3">
-        <f t="shared" ref="Q28" si="29">Q8-Q27</f>
+        <v>-757.63000000000011</v>
+      </c>
+      <c r="P29" s="30">
+        <f t="shared" ref="P29" si="28">P8-P28</f>
+        <v>-695.24599999999919</v>
+      </c>
+      <c r="Q29" s="3">
+        <f t="shared" ref="Q29" si="29">Q8-Q28</f>
         <v>2412.37</v>
       </c>
-      <c r="R28" s="3">
-        <f t="shared" ref="R28" si="30">R8-R27</f>
+      <c r="R29" s="3">
+        <f t="shared" ref="R29" si="30">R8-R28</f>
         <v>2412.37</v>
       </c>
-      <c r="S28" s="3">
-        <f t="shared" ref="S28" si="31">S8-S27</f>
+      <c r="S29" s="3">
+        <f t="shared" ref="S29" si="31">S8-S28</f>
         <v>2412.37</v>
       </c>
-      <c r="T28" s="3">
-        <f t="shared" ref="T28" si="32">T8-T27</f>
+      <c r="T29" s="3">
+        <f t="shared" ref="T29" si="32">T8-T28</f>
         <v>2412.37</v>
       </c>
-      <c r="U28" s="3">
-        <f t="shared" ref="U28" si="33">U8-U27</f>
+      <c r="U29" s="3">
+        <f t="shared" ref="U29" si="33">U8-U28</f>
         <v>2412.37</v>
       </c>
-      <c r="V28" s="3">
-        <f t="shared" ref="V28" si="34">V8-V27</f>
+      <c r="V29" s="3">
+        <f t="shared" ref="V29" si="34">V8-V28</f>
         <v>-2337.630000000001</v>
       </c>
-      <c r="W28" s="3">
-        <f t="shared" ref="W28" si="35">W8-W27</f>
+      <c r="W29" s="3">
+        <f t="shared" ref="W29" si="35">W8-W28</f>
         <v>2912.37</v>
       </c>
-      <c r="X28" s="3">
-        <f t="shared" ref="X28" si="36">X8-X27</f>
+      <c r="X29" s="3">
+        <f t="shared" ref="X29" si="36">X8-X28</f>
         <v>2912.37</v>
       </c>
-      <c r="Y28" s="3">
-        <f t="shared" ref="Y28" si="37">Y8-Y27</f>
+      <c r="Y29" s="3">
+        <f t="shared" ref="Y29" si="37">Y8-Y28</f>
         <v>2912.37</v>
       </c>
-      <c r="Z28" s="3">
-        <f t="shared" ref="Z28" si="38">Z8-Z27</f>
+      <c r="Z29" s="3">
+        <f t="shared" ref="Z29" si="38">Z8-Z28</f>
         <v>2912.37</v>
       </c>
-      <c r="AA28" s="31">
-        <f t="shared" ref="AA28" si="39">AA8-AA27</f>
-        <v>2047.37</v>
-      </c>
-      <c r="AB28" s="30">
-        <f t="shared" ref="AB28" si="40">AB8-AB27</f>
-        <v>-10987.630000000001</v>
-      </c>
-      <c r="AC28" s="3">
-        <f t="shared" ref="AC28" si="41">AC8-AC27</f>
+      <c r="AA29" s="31">
+        <f t="shared" ref="AA29" si="39">AA8-AA28</f>
+        <v>-7952.630000000001</v>
+      </c>
+      <c r="AB29" s="30">
+        <f t="shared" ref="AB29" si="40">AB8-AB28</f>
+        <v>-7635.5755999999965</v>
+      </c>
+      <c r="AC29" s="3">
+        <f t="shared" ref="AC29" si="41">AC8-AC28</f>
         <v>112.3700000000008</v>
       </c>
-      <c r="AD28" s="3">
-        <f t="shared" ref="AD28" si="42">AD8-AD27</f>
+      <c r="AD29" s="3">
+        <f t="shared" ref="AD29" si="42">AD8-AD28</f>
         <v>112.3700000000008</v>
       </c>
-      <c r="AE28" s="3">
-        <f t="shared" ref="AE28" si="43">AE8-AE27</f>
+      <c r="AE29" s="3">
+        <f t="shared" ref="AE29" si="43">AE8-AE28</f>
         <v>112.3700000000008</v>
       </c>
-      <c r="AF28" s="3">
-        <f t="shared" ref="AF28" si="44">AF8-AF27</f>
+      <c r="AF29" s="3">
+        <f t="shared" ref="AF29" si="44">AF8-AF28</f>
         <v>112.3700000000008</v>
       </c>
-      <c r="AG28" s="3">
-        <f t="shared" ref="AG28" si="45">AG8-AG27</f>
+      <c r="AG29" s="3">
+        <f t="shared" ref="AG29" si="45">AG8-AG28</f>
         <v>112.3700000000008</v>
       </c>
-      <c r="AH28" s="3">
-        <f t="shared" ref="AH28" si="46">AH8-AH27</f>
-        <v>-9587.630000000001</v>
-      </c>
-      <c r="AI28" s="3">
-        <f t="shared" ref="AI28" si="47">AI8-AI27</f>
+      <c r="AH29" s="3">
+        <f t="shared" ref="AH29" si="46">AH8-AH28</f>
+        <v>412.3700000000008</v>
+      </c>
+      <c r="AI29" s="3">
+        <f t="shared" ref="AI29" si="47">AI8-AI28</f>
         <v>712.3700000000008</v>
       </c>
-      <c r="AJ28" s="3">
-        <f t="shared" ref="AJ28" si="48">AJ8-AJ27</f>
+      <c r="AJ29" s="3">
+        <f t="shared" ref="AJ29" si="48">AJ8-AJ28</f>
         <v>712.3700000000008</v>
       </c>
-      <c r="AK28" s="3">
-        <f t="shared" ref="AK28" si="49">AK8-AK27</f>
+      <c r="AK29" s="3">
+        <f t="shared" ref="AK29" si="49">AK8-AK28</f>
         <v>712.3700000000008</v>
       </c>
-      <c r="AL28" s="3">
-        <f t="shared" ref="AL28" si="50">AL8-AL27</f>
+      <c r="AL29" s="3">
+        <f t="shared" ref="AL29" si="50">AL8-AL28</f>
         <v>712.3700000000008</v>
       </c>
-      <c r="AM28" s="31">
-        <f t="shared" ref="AM28" si="51">AM8-AM27</f>
+      <c r="AM29" s="31">
+        <f t="shared" ref="AM29" si="51">AM8-AM28</f>
         <v>297.3700000000008</v>
       </c>
     </row>
-    <row r="29" spans="1:39">
-      <c r="A29" s="4"/>
-      <c r="B29" s="32" t="s">
+    <row r="30" spans="1:39">
+      <c r="A30" s="4"/>
+      <c r="B30" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="95">
-        <f>C28</f>
+      <c r="C30" s="85">
+        <f>C29</f>
         <v>260.70000000000005</v>
       </c>
-      <c r="D29" s="32">
-        <f t="shared" ref="D29:O29" si="52">C29+D28</f>
+      <c r="D30" s="32">
+        <f t="shared" ref="D30:O30" si="52">C30+D29</f>
         <v>277.96999999999997</v>
       </c>
-      <c r="E29" s="33">
+      <c r="E30" s="33">
         <f t="shared" si="52"/>
         <v>1385.34</v>
       </c>
-      <c r="F29" s="33">
+      <c r="F30" s="33">
         <f t="shared" si="52"/>
         <v>592.70999999999981</v>
       </c>
-      <c r="G29" s="33">
+      <c r="G30" s="33">
         <f t="shared" si="52"/>
         <v>500.0799999999997</v>
       </c>
-      <c r="H29" s="33">
+      <c r="H30" s="33">
         <f t="shared" si="52"/>
         <v>907.44999999999959</v>
       </c>
-      <c r="I29" s="33">
+      <c r="I30" s="33">
         <f t="shared" si="52"/>
         <v>1314.8199999999995</v>
       </c>
-      <c r="J29" s="33">
+      <c r="J30" s="33">
         <f t="shared" si="52"/>
         <v>1722.1899999999994</v>
       </c>
-      <c r="K29" s="33">
+      <c r="K30" s="33">
         <f t="shared" si="52"/>
         <v>2329.5599999999995</v>
       </c>
-      <c r="L29" s="33">
+      <c r="L30" s="33">
         <f t="shared" si="52"/>
         <v>3136.9299999999994</v>
       </c>
-      <c r="M29" s="33">
+      <c r="M30" s="33">
         <f t="shared" si="52"/>
         <v>3844.2999999999993</v>
       </c>
-      <c r="N29" s="33">
+      <c r="N30" s="33">
         <f t="shared" si="52"/>
         <v>4651.6699999999992</v>
       </c>
-      <c r="O29" s="34">
+      <c r="O30" s="34">
         <f t="shared" si="52"/>
-        <v>4894.0399999999991</v>
-      </c>
-      <c r="P29" s="32">
-        <f t="shared" ref="P29" si="53">O29+P28</f>
-        <v>4756.4099999999989</v>
-      </c>
-      <c r="Q29" s="33">
-        <f t="shared" ref="Q29" si="54">P29+Q28</f>
-        <v>7168.7799999999988</v>
-      </c>
-      <c r="R29" s="33">
-        <f t="shared" ref="R29" si="55">Q29+R28</f>
-        <v>9581.1499999999978</v>
-      </c>
-      <c r="S29" s="33">
-        <f t="shared" ref="S29" si="56">R29+S28</f>
-        <v>11993.519999999997</v>
-      </c>
-      <c r="T29" s="33">
-        <f t="shared" ref="T29" si="57">S29+T28</f>
-        <v>14405.889999999996</v>
-      </c>
-      <c r="U29" s="33">
-        <f t="shared" ref="U29" si="58">T29+U28</f>
-        <v>16818.259999999995</v>
-      </c>
-      <c r="V29" s="33">
-        <f t="shared" ref="V29" si="59">U29+V28</f>
-        <v>14480.629999999994</v>
-      </c>
-      <c r="W29" s="33">
-        <f t="shared" ref="W29" si="60">V29+W28</f>
-        <v>17392.999999999993</v>
-      </c>
-      <c r="X29" s="33">
-        <f t="shared" ref="X29" si="61">W29+X28</f>
-        <v>20305.369999999992</v>
-      </c>
-      <c r="Y29" s="33">
-        <f t="shared" ref="Y29" si="62">X29+Y28</f>
-        <v>23217.739999999991</v>
-      </c>
-      <c r="Z29" s="33">
-        <f t="shared" ref="Z29" si="63">Y29+Z28</f>
-        <v>26130.10999999999</v>
-      </c>
-      <c r="AA29" s="34">
-        <f t="shared" ref="AA29" si="64">Z29+AA28</f>
-        <v>28177.479999999989</v>
-      </c>
-      <c r="AB29" s="32">
-        <f t="shared" ref="AB29" si="65">AA29+AB28</f>
-        <v>17189.849999999988</v>
-      </c>
-      <c r="AC29" s="33">
-        <f t="shared" ref="AC29" si="66">AB29+AC28</f>
-        <v>17302.219999999987</v>
-      </c>
-      <c r="AD29" s="33">
-        <f t="shared" ref="AD29" si="67">AC29+AD28</f>
-        <v>17414.589999999989</v>
-      </c>
-      <c r="AE29" s="33">
-        <f t="shared" ref="AE29" si="68">AD29+AE28</f>
-        <v>17526.959999999992</v>
-      </c>
-      <c r="AF29" s="33">
-        <f t="shared" ref="AF29" si="69">AE29+AF28</f>
-        <v>17639.329999999994</v>
-      </c>
-      <c r="AG29" s="33">
-        <f t="shared" ref="AG29" si="70">AF29+AG28</f>
-        <v>17751.699999999997</v>
-      </c>
-      <c r="AH29" s="33">
-        <f t="shared" ref="AH29" si="71">AG29+AH28</f>
-        <v>8164.0699999999961</v>
-      </c>
-      <c r="AI29" s="33">
-        <f t="shared" ref="AI29" si="72">AH29+AI28</f>
-        <v>8876.4399999999969</v>
-      </c>
-      <c r="AJ29" s="33">
-        <f t="shared" ref="AJ29" si="73">AI29+AJ28</f>
-        <v>9588.8099999999977</v>
-      </c>
-      <c r="AK29" s="33">
-        <f t="shared" ref="AK29" si="74">AJ29+AK28</f>
-        <v>10301.179999999998</v>
-      </c>
-      <c r="AL29" s="33">
-        <f t="shared" ref="AL29" si="75">AK29+AL28</f>
-        <v>11013.55</v>
-      </c>
-      <c r="AM29" s="34">
-        <f t="shared" ref="AM29" si="76">AL29+AM28</f>
-        <v>11310.92</v>
+        <v>3894.0399999999991</v>
+      </c>
+      <c r="P30" s="32">
+        <f t="shared" ref="P30" si="53">O30+P29</f>
+        <v>3198.7939999999999</v>
+      </c>
+      <c r="Q30" s="33">
+        <f t="shared" ref="Q30" si="54">P30+Q29</f>
+        <v>5611.1639999999998</v>
+      </c>
+      <c r="R30" s="33">
+        <f t="shared" ref="R30" si="55">Q30+R29</f>
+        <v>8023.5339999999997</v>
+      </c>
+      <c r="S30" s="33">
+        <f t="shared" ref="S30" si="56">R30+S29</f>
+        <v>10435.903999999999</v>
+      </c>
+      <c r="T30" s="33">
+        <f t="shared" ref="T30" si="57">S30+T29</f>
+        <v>12848.273999999998</v>
+      </c>
+      <c r="U30" s="33">
+        <f t="shared" ref="U30" si="58">T30+U29</f>
+        <v>15260.643999999997</v>
+      </c>
+      <c r="V30" s="33">
+        <f t="shared" ref="V30" si="59">U30+V29</f>
+        <v>12923.013999999996</v>
+      </c>
+      <c r="W30" s="33">
+        <f t="shared" ref="W30" si="60">V30+W29</f>
+        <v>15835.383999999995</v>
+      </c>
+      <c r="X30" s="33">
+        <f t="shared" ref="X30" si="61">W30+X29</f>
+        <v>18747.753999999994</v>
+      </c>
+      <c r="Y30" s="33">
+        <f t="shared" ref="Y30" si="62">X30+Y29</f>
+        <v>21660.123999999993</v>
+      </c>
+      <c r="Z30" s="33">
+        <f t="shared" ref="Z30" si="63">Y30+Z29</f>
+        <v>24572.493999999992</v>
+      </c>
+      <c r="AA30" s="34">
+        <f t="shared" ref="AA30" si="64">Z30+AA29</f>
+        <v>16619.86399999999</v>
+      </c>
+      <c r="AB30" s="32">
+        <f t="shared" ref="AB30" si="65">AA30+AB29</f>
+        <v>8984.288399999994</v>
+      </c>
+      <c r="AC30" s="33">
+        <f t="shared" ref="AC30" si="66">AB30+AC29</f>
+        <v>9096.6583999999948</v>
+      </c>
+      <c r="AD30" s="33">
+        <f t="shared" ref="AD30" si="67">AC30+AD29</f>
+        <v>9209.0283999999956</v>
+      </c>
+      <c r="AE30" s="33">
+        <f t="shared" ref="AE30" si="68">AD30+AE29</f>
+        <v>9321.3983999999964</v>
+      </c>
+      <c r="AF30" s="33">
+        <f t="shared" ref="AF30" si="69">AE30+AF29</f>
+        <v>9433.7683999999972</v>
+      </c>
+      <c r="AG30" s="33">
+        <f t="shared" ref="AG30" si="70">AF30+AG29</f>
+        <v>9546.138399999998</v>
+      </c>
+      <c r="AH30" s="33">
+        <f t="shared" ref="AH30" si="71">AG30+AH29</f>
+        <v>9958.5083999999988</v>
+      </c>
+      <c r="AI30" s="33">
+        <f t="shared" ref="AI30" si="72">AH30+AI29</f>
+        <v>10670.8784</v>
+      </c>
+      <c r="AJ30" s="33">
+        <f t="shared" ref="AJ30" si="73">AI30+AJ29</f>
+        <v>11383.2484</v>
+      </c>
+      <c r="AK30" s="33">
+        <f t="shared" ref="AK30" si="74">AJ30+AK29</f>
+        <v>12095.618400000001</v>
+      </c>
+      <c r="AL30" s="33">
+        <f t="shared" ref="AL30" si="75">AK30+AL29</f>
+        <v>12807.988400000002</v>
+      </c>
+      <c r="AM30" s="34">
+        <f t="shared" ref="AM30" si="76">AL30+AM29</f>
+        <v>13105.358400000003</v>
       </c>
     </row>
   </sheetData>
@@ -4381,7 +4461,7 @@
     <mergeCell ref="P9:AA9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="C28:AM29">
+  <conditionalFormatting sqref="C29:AM30">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -4532,48 +4612,48 @@
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
       <c r="A2" s="23"/>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="82"/>
-      <c r="N2" s="80" t="s">
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="94"/>
+      <c r="N2" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="81"/>
-      <c r="R2" s="81"/>
-      <c r="S2" s="81"/>
-      <c r="T2" s="81"/>
-      <c r="U2" s="81"/>
-      <c r="V2" s="81"/>
-      <c r="W2" s="81"/>
-      <c r="X2" s="81"/>
-      <c r="Y2" s="82"/>
-      <c r="Z2" s="80" t="s">
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93"/>
+      <c r="S2" s="93"/>
+      <c r="T2" s="93"/>
+      <c r="U2" s="93"/>
+      <c r="V2" s="93"/>
+      <c r="W2" s="93"/>
+      <c r="X2" s="93"/>
+      <c r="Y2" s="94"/>
+      <c r="Z2" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="AA2" s="81"/>
-      <c r="AB2" s="81"/>
-      <c r="AC2" s="81"/>
-      <c r="AD2" s="81"/>
-      <c r="AE2" s="81"/>
-      <c r="AF2" s="81"/>
-      <c r="AG2" s="81"/>
-      <c r="AH2" s="81"/>
-      <c r="AI2" s="81"/>
-      <c r="AJ2" s="81"/>
-      <c r="AK2" s="82"/>
+      <c r="AA2" s="93"/>
+      <c r="AB2" s="93"/>
+      <c r="AC2" s="93"/>
+      <c r="AD2" s="93"/>
+      <c r="AE2" s="93"/>
+      <c r="AF2" s="93"/>
+      <c r="AG2" s="93"/>
+      <c r="AH2" s="93"/>
+      <c r="AI2" s="93"/>
+      <c r="AJ2" s="93"/>
+      <c r="AK2" s="94"/>
     </row>
     <row r="3" spans="1:37" ht="15">
       <c r="A3" s="19" t="s">
@@ -7848,21 +7928,21 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
     </row>
     <row r="3" spans="1:14" ht="15">
       <c r="A3" s="12" t="s">

</xml_diff>

<commit_message>
corrections made to forecasting
</commit_message>
<xml_diff>
--- a/business plan/Cash Flow.xlsx
+++ b/business plan/Cash Flow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Financial Forecast" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
   <si>
     <t>Receipts</t>
   </si>
@@ -47,13 +47,7 @@
     <t>Total Expenses</t>
   </si>
   <si>
-    <t>net cash flow</t>
-  </si>
-  <si>
     <t>closing balance</t>
-  </si>
-  <si>
-    <t>start-up</t>
   </si>
   <si>
     <t>Business Space</t>
@@ -199,14 +193,27 @@
   <si>
     <t>Equipment</t>
   </si>
+  <si>
+    <t>Net Cash Flow</t>
+  </si>
+  <si>
+    <t>Corporation Tax</t>
+  </si>
+  <si>
+    <t>Cumulative Expenses</t>
+  </si>
+  <si>
+    <t>Cumulative Income</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$£-809]\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="[$£-809]#,##0.00"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -653,7 +660,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="98">
+  <cellStyleXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -752,8 +759,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1012,6 +1023,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1042,17 +1062,14 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="98">
+  <cellStyles count="102">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1101,6 +1118,8 @@
     <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1149,6 +1168,8 @@
     <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="63" builtinId="10"/>
   </cellStyles>
@@ -1173,6 +1194,1562 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.172574582014394"/>
+          <c:y val="0.0125386977799941"/>
+          <c:w val="0.826362860004973"/>
+          <c:h val="0.963312699088165"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Forecast'!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Receipts</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Financial Forecast'!$D$1:$O$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Forecast'!$D$8:$O$8</c:f>
+              <c:numCache>
+                <c:formatCode>[$£-809]\ #,##0.00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1600.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3100.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3600.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3600.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3600.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3800.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3900.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4300.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Forecast'!$B$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Expenses</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Financial Forecast'!$D$1:$O$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Forecast'!$D$28:$O$28</c:f>
+              <c:numCache>
+                <c:formatCode>[$£-809]\ #,##0.00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>482.7300000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>492.6300000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3192.63</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3192.63</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3192.63</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3192.63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3192.63</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3192.63</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3192.63</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3192.63</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3192.63</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5057.63</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Forecast'!$B$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Net Cash Flow</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Financial Forecast'!$D$1:$O$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Forecast'!$D$29:$O$29</c:f>
+              <c:numCache>
+                <c:formatCode>[$£-809]\ #,##0.00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>17.26999999999992</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1107.37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-792.6300000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-92.63000000000011</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>407.3699999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>407.3699999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>407.3699999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>607.3699999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>807.3699999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>707.3699999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>807.3699999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-757.6300000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Forecast'!$B$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>closing balance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Financial Forecast'!$D$1:$O$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Forecast'!$D$30:$O$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>-722.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>385.3399999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-407.2900000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-499.9200000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-92.55000000000041</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>314.8199999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>722.1899999999993</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1329.559999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2136.929999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2844.299999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3651.669999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2894.04</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2147285992"/>
+        <c:axId val="2112283864"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2147285992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2112283864"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2112283864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="[$£-809]\ #,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2147285992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Forecast'!$B$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cumulative Expenses</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Forecast'!$C$32:$O$32</c:f>
+              <c:numCache>
+                <c:formatCode>[$£-809]#,##0.00</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0" formatCode="[$£-809]\ #,##0.00">
+                  <c:v>1639.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2122.03</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2614.66</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5807.290000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8999.920000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12192.55</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15385.18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18577.81</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21770.44000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24963.07000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28155.70000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>31348.33000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>36405.96000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Forecast'!$B$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cumulative Income</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Forecast'!$C$33:$O$33</c:f>
+              <c:numCache>
+                <c:formatCode>[$£-809]#,##0.00</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0" formatCode="[$£-809]\ #,##0.00">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1400.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5400.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12100.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15700.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19300.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23100.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27100.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>31000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>35000.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39300.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2139618968"/>
+        <c:axId val="-2142688216"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2139618968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2142688216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2142688216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="[$£-809]\ #,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2139618968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Forecast'!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Receipts</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Forecast'!$C$8:$AM$8</c:f>
+              <c:numCache>
+                <c:formatCode>[$£-809]\ #,##0.00</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1600.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3100.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3600.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3600.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3600.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3800.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3900.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4300.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5950.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7750.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9100.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10200.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10200.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10200.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10200.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>10200.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>10500.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10800.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>10800.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>10800.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>10800.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>10800.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Forecast'!$B$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Expenses</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Forecast'!$C$28:$AM$28</c:f>
+              <c:numCache>
+                <c:formatCode>[$£-809]\ #,##0.00</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>1639.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>482.7300000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>492.6300000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3192.63</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3192.63</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3192.63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3192.63</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3192.63</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3192.63</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3192.63</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3192.63</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3192.63</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5057.63</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5666.438</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5087.63</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5087.63</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5087.63</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5087.63</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5087.63</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5087.63</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5087.63</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5087.63</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5087.63</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5087.63</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>15952.63</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>14407.3644</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10087.63</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10087.63</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10087.63</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10087.63</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>10087.63</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>10087.63</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10087.63</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>10087.63</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>10087.63</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>10087.63</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>10502.63</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Forecast'!$B$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Net Cash Flow</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Forecast'!$C$29:$AM$29</c:f>
+              <c:numCache>
+                <c:formatCode>[$£-809]\ #,##0.00</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>-739.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.26999999999992</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1107.37</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-792.6300000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-92.63000000000011</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>407.3699999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>407.3699999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>407.3699999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>607.3699999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>807.3699999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>707.3699999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>807.3699999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-757.6300000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>283.5619999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2412.37</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2412.37</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2412.37</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2412.37</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2412.37</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2662.37</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2912.37</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2912.37</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2912.37</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2912.37</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-7952.630000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-5307.364399999998</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>112.3700000000008</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>112.3700000000008</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>112.3700000000008</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>112.3700000000008</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>112.3700000000008</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>412.3700000000008</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>712.3700000000008</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>712.3700000000008</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>712.3700000000008</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>712.3700000000008</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>297.3700000000008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Forecast'!$B$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>closing balance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Forecast'!$C$30:$AM$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>-739.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-722.03</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>385.3399999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-407.2900000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-499.9200000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-92.55000000000041</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>314.8199999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>722.1899999999993</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1329.559999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2136.929999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2844.299999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3651.669999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2894.04</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3177.601999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5589.971999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8002.341999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10414.712</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12827.082</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15239.452</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>17901.822</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20814.192</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23726.56199999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>26638.93199999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>29551.30199999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>21598.67199999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>16291.30759999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>16403.6776</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>16516.0476</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>16628.4176</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>16740.7876</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>16853.15760000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>17265.52760000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>17977.89760000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>18690.26760000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>19402.63760000002</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>20115.00760000002</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>20412.37760000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2138847384"/>
+        <c:axId val="-2142719384"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2138847384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2142719384"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2142719384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="[$£-809]\ #,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2138847384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>338666</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>67734</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>118533</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>67734</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>592667</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>118533</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1295400</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1500,11 +3077,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:AM30"/>
+  <dimension ref="A1:AM33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AF1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P34" sqref="P34"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Z28" sqref="Z28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1518,8 +3095,8 @@
     <row r="1" spans="1:39" s="64" customFormat="1" ht="30" customHeight="1">
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
-      <c r="C1" s="77" t="s">
-        <v>9</v>
+      <c r="C1" s="77">
+        <v>0</v>
       </c>
       <c r="D1" s="58">
         <v>1</v>
@@ -1632,7 +3209,7 @@
     </row>
     <row r="2" spans="1:39" s="66" customFormat="1" ht="30" customHeight="1">
       <c r="A2" s="65" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="57" t="s">
         <v>0</v>
@@ -1640,55 +3217,55 @@
       <c r="C2" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="89" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="89" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="90"/>
-      <c r="S2" s="90"/>
-      <c r="T2" s="90"/>
-      <c r="U2" s="90"/>
-      <c r="V2" s="90"/>
-      <c r="W2" s="90"/>
-      <c r="X2" s="90"/>
-      <c r="Y2" s="90"/>
-      <c r="Z2" s="90"/>
-      <c r="AA2" s="91"/>
-      <c r="AB2" s="89" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="90"/>
-      <c r="AD2" s="90"/>
-      <c r="AE2" s="90"/>
-      <c r="AF2" s="90"/>
-      <c r="AG2" s="90"/>
-      <c r="AH2" s="90"/>
-      <c r="AI2" s="90"/>
-      <c r="AJ2" s="90"/>
-      <c r="AK2" s="90"/>
-      <c r="AL2" s="90"/>
-      <c r="AM2" s="91"/>
+      <c r="D2" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="94"/>
+      <c r="P2" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93"/>
+      <c r="S2" s="93"/>
+      <c r="T2" s="93"/>
+      <c r="U2" s="93"/>
+      <c r="V2" s="93"/>
+      <c r="W2" s="93"/>
+      <c r="X2" s="93"/>
+      <c r="Y2" s="93"/>
+      <c r="Z2" s="93"/>
+      <c r="AA2" s="94"/>
+      <c r="AB2" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="93"/>
+      <c r="AD2" s="93"/>
+      <c r="AE2" s="93"/>
+      <c r="AF2" s="93"/>
+      <c r="AG2" s="93"/>
+      <c r="AH2" s="93"/>
+      <c r="AI2" s="93"/>
+      <c r="AJ2" s="93"/>
+      <c r="AK2" s="93"/>
+      <c r="AL2" s="93"/>
+      <c r="AM2" s="94"/>
     </row>
     <row r="3" spans="1:39" s="67" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="79"/>
       <c r="D3" s="24">
@@ -1802,10 +3379,10 @@
     </row>
     <row r="4" spans="1:39" s="67" customFormat="1">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="79"/>
       <c r="D4" s="24">
@@ -1919,10 +3496,10 @@
     </row>
     <row r="5" spans="1:39" s="67" customFormat="1">
       <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="35" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" s="35" t="s">
-        <v>16</v>
       </c>
       <c r="C5" s="79"/>
       <c r="D5" s="24">
@@ -2036,10 +3613,10 @@
     </row>
     <row r="6" spans="1:39" s="67" customFormat="1">
       <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="35" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>17</v>
       </c>
       <c r="C6" s="79"/>
       <c r="D6" s="24">
@@ -2153,10 +3730,10 @@
     </row>
     <row r="7" spans="1:39" s="67" customFormat="1">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7" s="79">
         <v>900</v>
@@ -2360,55 +3937,55 @@
       <c r="C9" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="86" t="s">
+      <c r="D9" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="87"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="87"/>
-      <c r="H9" s="87"/>
-      <c r="I9" s="87"/>
-      <c r="J9" s="87"/>
-      <c r="K9" s="87"/>
-      <c r="L9" s="87"/>
-      <c r="M9" s="87"/>
-      <c r="N9" s="87"/>
-      <c r="O9" s="88"/>
-      <c r="P9" s="86" t="s">
+      <c r="E9" s="90"/>
+      <c r="F9" s="90"/>
+      <c r="G9" s="90"/>
+      <c r="H9" s="90"/>
+      <c r="I9" s="90"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="90"/>
+      <c r="M9" s="90"/>
+      <c r="N9" s="90"/>
+      <c r="O9" s="91"/>
+      <c r="P9" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="Q9" s="87"/>
-      <c r="R9" s="87"/>
-      <c r="S9" s="87"/>
-      <c r="T9" s="87"/>
-      <c r="U9" s="87"/>
-      <c r="V9" s="87"/>
-      <c r="W9" s="87"/>
-      <c r="X9" s="87"/>
-      <c r="Y9" s="87"/>
-      <c r="Z9" s="87"/>
-      <c r="AA9" s="88"/>
-      <c r="AB9" s="86" t="s">
+      <c r="Q9" s="90"/>
+      <c r="R9" s="90"/>
+      <c r="S9" s="90"/>
+      <c r="T9" s="90"/>
+      <c r="U9" s="90"/>
+      <c r="V9" s="90"/>
+      <c r="W9" s="90"/>
+      <c r="X9" s="90"/>
+      <c r="Y9" s="90"/>
+      <c r="Z9" s="90"/>
+      <c r="AA9" s="91"/>
+      <c r="AB9" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="AC9" s="87"/>
-      <c r="AD9" s="87"/>
-      <c r="AE9" s="87"/>
-      <c r="AF9" s="87"/>
-      <c r="AG9" s="87"/>
-      <c r="AH9" s="87"/>
-      <c r="AI9" s="87"/>
-      <c r="AJ9" s="87"/>
-      <c r="AK9" s="87"/>
-      <c r="AL9" s="87"/>
-      <c r="AM9" s="88"/>
+      <c r="AC9" s="90"/>
+      <c r="AD9" s="90"/>
+      <c r="AE9" s="90"/>
+      <c r="AF9" s="90"/>
+      <c r="AG9" s="90"/>
+      <c r="AH9" s="90"/>
+      <c r="AI9" s="90"/>
+      <c r="AJ9" s="90"/>
+      <c r="AK9" s="90"/>
+      <c r="AL9" s="90"/>
+      <c r="AM9" s="91"/>
     </row>
     <row r="10" spans="1:39" s="70" customFormat="1">
       <c r="A10" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" s="82"/>
       <c r="D10" s="28">
@@ -2523,7 +4100,7 @@
     <row r="11" spans="1:39" s="70" customFormat="1">
       <c r="A11" s="5"/>
       <c r="B11" s="37" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C11" s="82"/>
       <c r="D11" s="28">
@@ -2637,10 +4214,10 @@
     </row>
     <row r="12" spans="1:39" s="70" customFormat="1">
       <c r="A12" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="82">
         <v>60.8</v>
@@ -2759,7 +4336,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" s="82"/>
       <c r="D13" s="28">
@@ -2873,10 +4450,10 @@
     </row>
     <row r="14" spans="1:39" s="70" customFormat="1">
       <c r="A14" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" s="82">
         <v>7</v>
@@ -2920,10 +4497,10 @@
     </row>
     <row r="15" spans="1:39" s="70" customFormat="1">
       <c r="A15" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" s="82"/>
       <c r="D15" s="28">
@@ -3076,7 +4653,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16" s="82"/>
       <c r="D16" s="28">
@@ -3190,10 +4767,10 @@
     </row>
     <row r="17" spans="1:39" s="70" customFormat="1">
       <c r="A17" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C17" s="82">
         <v>11.5</v>
@@ -3310,7 +4887,7 @@
     <row r="18" spans="1:39" s="70" customFormat="1">
       <c r="A18" s="5"/>
       <c r="B18" s="37" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C18" s="82"/>
       <c r="D18" s="28"/>
@@ -3323,27 +4900,25 @@
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
-      <c r="N18" s="96"/>
-      <c r="O18" s="98">
+      <c r="N18" s="86"/>
+      <c r="O18" s="87">
         <v>1000</v>
       </c>
-      <c r="P18" s="97"/>
+      <c r="P18" s="87"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
       <c r="T18" s="6"/>
       <c r="U18" s="6"/>
-      <c r="V18" s="6">
-        <v>5000</v>
-      </c>
+      <c r="V18" s="6"/>
       <c r="W18" s="6"/>
       <c r="X18" s="6"/>
       <c r="Y18" s="6"/>
-      <c r="Z18" s="96"/>
-      <c r="AA18" s="98">
+      <c r="Z18" s="86"/>
+      <c r="AA18" s="88">
         <v>10000</v>
       </c>
-      <c r="AB18" s="97"/>
+      <c r="AB18" s="87"/>
       <c r="AC18" s="6"/>
       <c r="AD18" s="6"/>
       <c r="AE18" s="6"/>
@@ -3358,10 +4933,10 @@
     </row>
     <row r="19" spans="1:39" s="70" customFormat="1">
       <c r="A19" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C19" s="82">
         <v>50</v>
@@ -3405,10 +4980,10 @@
     </row>
     <row r="20" spans="1:39" s="70" customFormat="1">
       <c r="A20" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C20" s="82"/>
       <c r="D20" s="28">
@@ -3522,10 +5097,10 @@
     </row>
     <row r="21" spans="1:39" s="70" customFormat="1">
       <c r="A21" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C21" s="82">
         <v>10</v>
@@ -3569,10 +5144,10 @@
     </row>
     <row r="22" spans="1:39" s="70" customFormat="1">
       <c r="A22" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B22" s="37" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C22" s="82"/>
       <c r="D22" s="28">
@@ -3686,10 +5261,10 @@
     </row>
     <row r="23" spans="1:39" s="70" customFormat="1">
       <c r="A23" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C23" s="82"/>
       <c r="D23" s="63"/>
@@ -3741,7 +5316,7 @@
         <v>5</v>
       </c>
       <c r="C24" s="83">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="D24" s="74"/>
       <c r="E24" s="75"/>
@@ -3783,7 +5358,7 @@
     <row r="25" spans="1:39" s="70" customFormat="1">
       <c r="A25" s="5"/>
       <c r="B25" s="37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C25" s="82"/>
       <c r="D25" s="63"/>
@@ -3829,7 +5404,9 @@
     </row>
     <row r="26" spans="1:39" s="70" customFormat="1">
       <c r="A26" s="5"/>
-      <c r="B26" s="37"/>
+      <c r="B26" s="37" t="s">
+        <v>57</v>
+      </c>
       <c r="C26" s="82"/>
       <c r="D26" s="63"/>
       <c r="E26" s="73"/>
@@ -3844,8 +5421,8 @@
       <c r="N26" s="73"/>
       <c r="O26" s="71"/>
       <c r="P26" s="63">
-        <f>SUM(0.4*O30)</f>
-        <v>1557.6159999999998</v>
+        <f>SUM(0.2*O30)</f>
+        <v>578.80799999999988</v>
       </c>
       <c r="Q26" s="73"/>
       <c r="R26" s="73"/>
@@ -3859,8 +5436,8 @@
       <c r="Z26" s="73"/>
       <c r="AA26" s="71"/>
       <c r="AB26" s="63">
-        <f>SUM(0.4*AA30)</f>
-        <v>6647.9455999999964</v>
+        <f>SUM(0.2*AA30)</f>
+        <v>4319.7343999999985</v>
       </c>
       <c r="AC26" s="73"/>
       <c r="AD26" s="73"/>
@@ -3877,7 +5454,7 @@
     <row r="27" spans="1:39" s="70" customFormat="1">
       <c r="A27" s="5"/>
       <c r="B27" s="37" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C27" s="82"/>
       <c r="D27" s="28">
@@ -3996,7 +5573,7 @@
       </c>
       <c r="C28" s="80">
         <f t="shared" ref="C28:O28" si="2">SUM(C9:C27)</f>
-        <v>639.29999999999995</v>
+        <v>1639.3</v>
       </c>
       <c r="D28" s="26">
         <f t="shared" si="2"/>
@@ -4048,7 +5625,7 @@
       </c>
       <c r="P28" s="26">
         <f t="shared" ref="P28" si="3">SUM(P9:P27)</f>
-        <v>6645.2459999999992</v>
+        <v>5666.4380000000001</v>
       </c>
       <c r="Q28" s="8">
         <f t="shared" ref="Q28" si="4">SUM(Q9:Q27)</f>
@@ -4072,7 +5649,7 @@
       </c>
       <c r="V28" s="8">
         <f t="shared" ref="V28" si="9">SUM(V9:V27)</f>
-        <v>10087.630000000001</v>
+        <v>5087.63</v>
       </c>
       <c r="W28" s="8">
         <f t="shared" ref="W28" si="10">SUM(W9:W27)</f>
@@ -4096,7 +5673,7 @@
       </c>
       <c r="AB28" s="26">
         <f t="shared" ref="AB28" si="15">SUM(AB9:AB27)</f>
-        <v>16735.575599999996</v>
+        <v>14407.364399999999</v>
       </c>
       <c r="AC28" s="8">
         <f t="shared" ref="AC28" si="16">SUM(AC9:AC27)</f>
@@ -4146,11 +5723,11 @@
     <row r="29" spans="1:39">
       <c r="A29" s="2"/>
       <c r="B29" s="38" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="C29" s="84">
         <f t="shared" ref="C29:O29" si="27">C8-C28</f>
-        <v>260.70000000000005</v>
+        <v>-739.3</v>
       </c>
       <c r="D29" s="30">
         <f t="shared" si="27"/>
@@ -4202,7 +5779,7 @@
       </c>
       <c r="P29" s="30">
         <f t="shared" ref="P29" si="28">P8-P28</f>
-        <v>-695.24599999999919</v>
+        <v>283.5619999999999</v>
       </c>
       <c r="Q29" s="3">
         <f t="shared" ref="Q29" si="29">Q8-Q28</f>
@@ -4226,7 +5803,7 @@
       </c>
       <c r="V29" s="3">
         <f t="shared" ref="V29" si="34">V8-V28</f>
-        <v>-2337.630000000001</v>
+        <v>2662.37</v>
       </c>
       <c r="W29" s="3">
         <f t="shared" ref="W29" si="35">W8-W28</f>
@@ -4250,7 +5827,7 @@
       </c>
       <c r="AB29" s="30">
         <f t="shared" ref="AB29" si="40">AB8-AB28</f>
-        <v>-7635.5755999999965</v>
+        <v>-5307.3643999999986</v>
       </c>
       <c r="AC29" s="3">
         <f t="shared" ref="AC29" si="41">AC8-AC28</f>
@@ -4300,155 +5877,269 @@
     <row r="30" spans="1:39">
       <c r="A30" s="4"/>
       <c r="B30" s="32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C30" s="85">
         <f>C29</f>
-        <v>260.70000000000005</v>
+        <v>-739.3</v>
       </c>
       <c r="D30" s="32">
         <f t="shared" ref="D30:O30" si="52">C30+D29</f>
-        <v>277.96999999999997</v>
+        <v>-722.03</v>
       </c>
       <c r="E30" s="33">
         <f t="shared" si="52"/>
-        <v>1385.34</v>
+        <v>385.33999999999992</v>
       </c>
       <c r="F30" s="33">
         <f t="shared" si="52"/>
-        <v>592.70999999999981</v>
+        <v>-407.29000000000019</v>
       </c>
       <c r="G30" s="33">
         <f t="shared" si="52"/>
-        <v>500.0799999999997</v>
+        <v>-499.9200000000003</v>
       </c>
       <c r="H30" s="33">
         <f t="shared" si="52"/>
-        <v>907.44999999999959</v>
+        <v>-92.550000000000409</v>
       </c>
       <c r="I30" s="33">
         <f t="shared" si="52"/>
-        <v>1314.8199999999995</v>
+        <v>314.81999999999948</v>
       </c>
       <c r="J30" s="33">
         <f t="shared" si="52"/>
-        <v>1722.1899999999994</v>
+        <v>722.18999999999937</v>
       </c>
       <c r="K30" s="33">
         <f t="shared" si="52"/>
-        <v>2329.5599999999995</v>
+        <v>1329.5599999999993</v>
       </c>
       <c r="L30" s="33">
         <f t="shared" si="52"/>
-        <v>3136.9299999999994</v>
+        <v>2136.9299999999994</v>
       </c>
       <c r="M30" s="33">
         <f t="shared" si="52"/>
-        <v>3844.2999999999993</v>
+        <v>2844.2999999999993</v>
       </c>
       <c r="N30" s="33">
         <f t="shared" si="52"/>
-        <v>4651.6699999999992</v>
+        <v>3651.6699999999992</v>
       </c>
       <c r="O30" s="34">
         <f t="shared" si="52"/>
-        <v>3894.0399999999991</v>
+        <v>2894.0399999999991</v>
       </c>
       <c r="P30" s="32">
         <f t="shared" ref="P30" si="53">O30+P29</f>
-        <v>3198.7939999999999</v>
+        <v>3177.601999999999</v>
       </c>
       <c r="Q30" s="33">
         <f t="shared" ref="Q30" si="54">P30+Q29</f>
-        <v>5611.1639999999998</v>
+        <v>5589.9719999999988</v>
       </c>
       <c r="R30" s="33">
         <f t="shared" ref="R30" si="55">Q30+R29</f>
-        <v>8023.5339999999997</v>
+        <v>8002.3419999999987</v>
       </c>
       <c r="S30" s="33">
         <f t="shared" ref="S30" si="56">R30+S29</f>
-        <v>10435.903999999999</v>
+        <v>10414.712</v>
       </c>
       <c r="T30" s="33">
         <f t="shared" ref="T30" si="57">S30+T29</f>
-        <v>12848.273999999998</v>
+        <v>12827.081999999999</v>
       </c>
       <c r="U30" s="33">
         <f t="shared" ref="U30" si="58">T30+U29</f>
-        <v>15260.643999999997</v>
+        <v>15239.451999999997</v>
       </c>
       <c r="V30" s="33">
         <f t="shared" ref="V30" si="59">U30+V29</f>
-        <v>12923.013999999996</v>
+        <v>17901.821999999996</v>
       </c>
       <c r="W30" s="33">
         <f t="shared" ref="W30" si="60">V30+W29</f>
-        <v>15835.383999999995</v>
+        <v>20814.191999999995</v>
       </c>
       <c r="X30" s="33">
         <f t="shared" ref="X30" si="61">W30+X29</f>
-        <v>18747.753999999994</v>
+        <v>23726.561999999994</v>
       </c>
       <c r="Y30" s="33">
         <f t="shared" ref="Y30" si="62">X30+Y29</f>
-        <v>21660.123999999993</v>
+        <v>26638.931999999993</v>
       </c>
       <c r="Z30" s="33">
         <f t="shared" ref="Z30" si="63">Y30+Z29</f>
-        <v>24572.493999999992</v>
+        <v>29551.301999999992</v>
       </c>
       <c r="AA30" s="34">
         <f t="shared" ref="AA30" si="64">Z30+AA29</f>
-        <v>16619.86399999999</v>
+        <v>21598.671999999991</v>
       </c>
       <c r="AB30" s="32">
         <f t="shared" ref="AB30" si="65">AA30+AB29</f>
-        <v>8984.288399999994</v>
+        <v>16291.307599999993</v>
       </c>
       <c r="AC30" s="33">
         <f t="shared" ref="AC30" si="66">AB30+AC29</f>
-        <v>9096.6583999999948</v>
+        <v>16403.677599999995</v>
       </c>
       <c r="AD30" s="33">
         <f t="shared" ref="AD30" si="67">AC30+AD29</f>
-        <v>9209.0283999999956</v>
+        <v>16516.047599999998</v>
       </c>
       <c r="AE30" s="33">
         <f t="shared" ref="AE30" si="68">AD30+AE29</f>
-        <v>9321.3983999999964</v>
+        <v>16628.417600000001</v>
       </c>
       <c r="AF30" s="33">
         <f t="shared" ref="AF30" si="69">AE30+AF29</f>
-        <v>9433.7683999999972</v>
+        <v>16740.787600000003</v>
       </c>
       <c r="AG30" s="33">
         <f t="shared" ref="AG30" si="70">AF30+AG29</f>
-        <v>9546.138399999998</v>
+        <v>16853.157600000006</v>
       </c>
       <c r="AH30" s="33">
         <f t="shared" ref="AH30" si="71">AG30+AH29</f>
-        <v>9958.5083999999988</v>
+        <v>17265.527600000009</v>
       </c>
       <c r="AI30" s="33">
         <f t="shared" ref="AI30" si="72">AH30+AI29</f>
-        <v>10670.8784</v>
+        <v>17977.897600000011</v>
       </c>
       <c r="AJ30" s="33">
         <f t="shared" ref="AJ30" si="73">AI30+AJ29</f>
-        <v>11383.2484</v>
+        <v>18690.267600000014</v>
       </c>
       <c r="AK30" s="33">
         <f t="shared" ref="AK30" si="74">AJ30+AK29</f>
-        <v>12095.618400000001</v>
+        <v>19402.637600000016</v>
       </c>
       <c r="AL30" s="33">
         <f t="shared" ref="AL30" si="75">AK30+AL29</f>
-        <v>12807.988400000002</v>
+        <v>20115.007600000019</v>
       </c>
       <c r="AM30" s="34">
         <f t="shared" ref="AM30" si="76">AL30+AM29</f>
-        <v>13105.358400000003</v>
+        <v>20412.377600000022</v>
+      </c>
+    </row>
+    <row r="32" spans="1:39">
+      <c r="B32" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="100">
+        <f>SUM(C28)</f>
+        <v>1639.3</v>
+      </c>
+      <c r="D32" s="99">
+        <f>SUM(C32+D28)</f>
+        <v>2122.0300000000002</v>
+      </c>
+      <c r="E32" s="99">
+        <f>SUM(D32+E28)</f>
+        <v>2614.6600000000003</v>
+      </c>
+      <c r="F32" s="99">
+        <f t="shared" ref="F32:O32" si="77">SUM(E32+F28)</f>
+        <v>5807.2900000000009</v>
+      </c>
+      <c r="G32" s="99">
+        <f t="shared" si="77"/>
+        <v>8999.9200000000019</v>
+      </c>
+      <c r="H32" s="99">
+        <f t="shared" si="77"/>
+        <v>12192.550000000003</v>
+      </c>
+      <c r="I32" s="99">
+        <f t="shared" si="77"/>
+        <v>15385.180000000004</v>
+      </c>
+      <c r="J32" s="99">
+        <f t="shared" si="77"/>
+        <v>18577.810000000005</v>
+      </c>
+      <c r="K32" s="99">
+        <f t="shared" si="77"/>
+        <v>21770.440000000006</v>
+      </c>
+      <c r="L32" s="99">
+        <f t="shared" si="77"/>
+        <v>24963.070000000007</v>
+      </c>
+      <c r="M32" s="99">
+        <f t="shared" si="77"/>
+        <v>28155.700000000008</v>
+      </c>
+      <c r="N32" s="99">
+        <f t="shared" si="77"/>
+        <v>31348.330000000009</v>
+      </c>
+      <c r="O32" s="99">
+        <f t="shared" si="77"/>
+        <v>36405.960000000006</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15">
+      <c r="B33" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="100">
+        <f>SUM(C8)</f>
+        <v>900</v>
+      </c>
+      <c r="D33" s="99">
+        <f>SUM(C33+D8)</f>
+        <v>1400</v>
+      </c>
+      <c r="E33" s="99">
+        <f t="shared" ref="E33:O33" si="78">SUM(D33+E8)</f>
+        <v>3000</v>
+      </c>
+      <c r="F33" s="99">
+        <f t="shared" si="78"/>
+        <v>5400</v>
+      </c>
+      <c r="G33" s="99">
+        <f t="shared" si="78"/>
+        <v>8500</v>
+      </c>
+      <c r="H33" s="99">
+        <f t="shared" si="78"/>
+        <v>12100</v>
+      </c>
+      <c r="I33" s="99">
+        <f t="shared" si="78"/>
+        <v>15700</v>
+      </c>
+      <c r="J33" s="99">
+        <f t="shared" si="78"/>
+        <v>19300</v>
+      </c>
+      <c r="K33" s="99">
+        <f t="shared" si="78"/>
+        <v>23100</v>
+      </c>
+      <c r="L33" s="99">
+        <f t="shared" si="78"/>
+        <v>27100</v>
+      </c>
+      <c r="M33" s="99">
+        <f t="shared" si="78"/>
+        <v>31000</v>
+      </c>
+      <c r="N33" s="99">
+        <f t="shared" si="78"/>
+        <v>35000</v>
+      </c>
+      <c r="O33" s="99">
+        <f t="shared" si="78"/>
+        <v>39300</v>
       </c>
     </row>
   </sheetData>
@@ -4474,6 +6165,7 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="5" max="1048575" man="1"/>
   </colBreaks>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>
@@ -4490,7 +6182,7 @@
   <dimension ref="A1:AK32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q41" sqref="Q41"/>
+      <selection activeCell="AC32" sqref="AC32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -4612,52 +6304,52 @@
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
       <c r="A2" s="23"/>
-      <c r="B2" s="92" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="93"/>
-      <c r="M2" s="94"/>
-      <c r="N2" s="92" t="s">
-        <v>37</v>
-      </c>
-      <c r="O2" s="93"/>
-      <c r="P2" s="93"/>
-      <c r="Q2" s="93"/>
-      <c r="R2" s="93"/>
-      <c r="S2" s="93"/>
-      <c r="T2" s="93"/>
-      <c r="U2" s="93"/>
-      <c r="V2" s="93"/>
-      <c r="W2" s="93"/>
-      <c r="X2" s="93"/>
-      <c r="Y2" s="94"/>
-      <c r="Z2" s="92" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA2" s="93"/>
-      <c r="AB2" s="93"/>
-      <c r="AC2" s="93"/>
-      <c r="AD2" s="93"/>
-      <c r="AE2" s="93"/>
-      <c r="AF2" s="93"/>
-      <c r="AG2" s="93"/>
-      <c r="AH2" s="93"/>
-      <c r="AI2" s="93"/>
-      <c r="AJ2" s="93"/>
-      <c r="AK2" s="94"/>
+      <c r="B2" s="95" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="95" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
+      <c r="Q2" s="96"/>
+      <c r="R2" s="96"/>
+      <c r="S2" s="96"/>
+      <c r="T2" s="96"/>
+      <c r="U2" s="96"/>
+      <c r="V2" s="96"/>
+      <c r="W2" s="96"/>
+      <c r="X2" s="96"/>
+      <c r="Y2" s="97"/>
+      <c r="Z2" s="95" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA2" s="96"/>
+      <c r="AB2" s="96"/>
+      <c r="AC2" s="96"/>
+      <c r="AD2" s="96"/>
+      <c r="AE2" s="96"/>
+      <c r="AF2" s="96"/>
+      <c r="AG2" s="96"/>
+      <c r="AH2" s="96"/>
+      <c r="AI2" s="96"/>
+      <c r="AJ2" s="96"/>
+      <c r="AK2" s="97"/>
     </row>
     <row r="3" spans="1:37" ht="15">
       <c r="A3" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" s="41">
         <v>200</v>
@@ -4770,7 +6462,7 @@
     </row>
     <row r="4" spans="1:37" ht="15">
       <c r="A4" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" s="43">
         <v>5</v>
@@ -4883,7 +6575,7 @@
     </row>
     <row r="5" spans="1:37" ht="15">
       <c r="A5" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B5" s="43">
         <f>SUM(B3*B4)</f>
@@ -5032,7 +6724,7 @@
     </row>
     <row r="6" spans="1:37" ht="15">
       <c r="A6" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" s="43">
         <f>SUM(B5/2)</f>
@@ -5181,7 +6873,7 @@
     </row>
     <row r="7" spans="1:37" ht="15">
       <c r="A7" s="21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" s="45">
         <v>400</v>
@@ -5294,7 +6986,7 @@
     </row>
     <row r="8" spans="1:37" ht="15">
       <c r="A8" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B8" s="45">
         <v>0</v>
@@ -5407,7 +7099,7 @@
     </row>
     <row r="9" spans="1:37" ht="15">
       <c r="A9" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="45">
         <v>0</v>
@@ -5555,7 +7247,7 @@
     </row>
     <row r="10" spans="1:37" ht="15">
       <c r="A10" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B10" s="45">
         <f>SUM(B8*300)</f>
@@ -5704,7 +7396,7 @@
     </row>
     <row r="11" spans="1:37" ht="15">
       <c r="A11" s="20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B11" s="43">
         <f t="shared" ref="B11:M11" si="4">SUM(B7)</f>
@@ -5853,7 +7545,7 @@
     </row>
     <row r="12" spans="1:37" ht="15">
       <c r="A12" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B12" s="43">
         <v>0</v>
@@ -5966,7 +7658,7 @@
     </row>
     <row r="13" spans="1:37" ht="15">
       <c r="A13" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B13" s="43">
         <v>0</v>
@@ -6114,7 +7806,7 @@
     </row>
     <row r="14" spans="1:37" ht="15">
       <c r="A14" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="43">
         <f>SUM(300*B12)</f>
@@ -6263,7 +7955,7 @@
     </row>
     <row r="15" spans="1:37" ht="15">
       <c r="A15" s="21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B15" s="45">
         <f t="shared" ref="B15:M15" si="8">SUM(B7)</f>
@@ -6412,7 +8104,7 @@
     </row>
     <row r="16" spans="1:37" ht="15">
       <c r="A16" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B16" s="45">
         <v>0</v>
@@ -6525,7 +8217,7 @@
     </row>
     <row r="17" spans="1:37" ht="15">
       <c r="A17" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B17" s="45">
         <v>0</v>
@@ -6673,7 +8365,7 @@
     </row>
     <row r="18" spans="1:37" ht="15">
       <c r="A18" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B18" s="45">
         <f>SUM(300*B16)</f>
@@ -6822,7 +8514,7 @@
     </row>
     <row r="19" spans="1:37" s="16" customFormat="1" ht="15">
       <c r="A19" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B19" s="47">
         <f t="shared" ref="B19:N19" si="12">SUM(B4+B8+B12+B16)</f>
@@ -6971,7 +8663,7 @@
     </row>
     <row r="20" spans="1:37" s="16" customFormat="1" ht="15">
       <c r="A20" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B20" s="47">
         <f t="shared" ref="B20:M20" si="14">SUM(B5+B9+B13+B17)</f>
@@ -7120,7 +8812,7 @@
     </row>
     <row r="21" spans="1:37" s="16" customFormat="1" ht="15">
       <c r="A21" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B21" s="49">
         <f t="shared" ref="B21:M21" si="16">SUM(B6+B10+B14+B18)</f>
@@ -7928,25 +9620,25 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15">
-      <c r="A2" s="95" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
+      <c r="A2" s="98" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
     </row>
     <row r="3" spans="1:14" ht="15">
       <c r="A3" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" s="13">
         <v>5</v>
@@ -7990,7 +9682,7 @@
     </row>
     <row r="4" spans="1:14" ht="15">
       <c r="A4" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B4" s="13">
         <f>SUM(N3*B3)</f>
@@ -8043,7 +9735,7 @@
     </row>
     <row r="5" spans="1:14" ht="15">
       <c r="A5" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" s="13">
         <f>SUM(B4/2)</f>
@@ -8096,7 +9788,7 @@
     </row>
     <row r="6" spans="1:14" ht="15">
       <c r="A6" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="15">
         <v>0</v>
@@ -8140,7 +9832,7 @@
     </row>
     <row r="7" spans="1:14" ht="15">
       <c r="A7" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B7" s="15">
         <v>0</v>
@@ -8192,7 +9884,7 @@
     </row>
     <row r="8" spans="1:14" ht="15">
       <c r="A8" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="15">
         <f>SUM(B6*300)</f>
@@ -8245,7 +9937,7 @@
     </row>
     <row r="9" spans="1:14" ht="15">
       <c r="A9" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" s="13">
         <v>0</v>
@@ -8286,7 +9978,7 @@
     </row>
     <row r="10" spans="1:14" ht="15">
       <c r="A10" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B10" s="13">
         <v>0</v>
@@ -8338,7 +10030,7 @@
     </row>
     <row r="11" spans="1:14" ht="15">
       <c r="A11" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="13">
         <f>SUM(300*B9)</f>
@@ -8391,7 +10083,7 @@
     </row>
     <row r="12" spans="1:14" ht="15">
       <c r="A12" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" s="15">
         <v>0</v>
@@ -8432,7 +10124,7 @@
     </row>
     <row r="13" spans="1:14" ht="15">
       <c r="A13" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B13" s="15">
         <v>0</v>
@@ -8484,7 +10176,7 @@
     </row>
     <row r="14" spans="1:14" ht="15">
       <c r="A14" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="15">
         <f>SUM(300*B12)</f>
@@ -8537,7 +10229,7 @@
     </row>
     <row r="15" spans="1:14" s="16" customFormat="1" ht="15">
       <c r="A15" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" s="11">
         <f>SUM(B3+B6+B9+B12)</f>
@@ -8590,7 +10282,7 @@
     </row>
     <row r="16" spans="1:14" s="16" customFormat="1" ht="15">
       <c r="A16" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" s="11">
         <f>SUM(B4+B7+B10+B13)</f>
@@ -8643,7 +10335,7 @@
     </row>
     <row r="17" spans="1:13" s="16" customFormat="1" ht="15">
       <c r="A17" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B17" s="11">
         <f>SUM(B5+B8+B11+B14)</f>

</xml_diff>